<commit_message>
wip mod timetable class
</commit_message>
<xml_diff>
--- a/csv/user.xlsx
+++ b/csv/user.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="461">
   <si>
     <t>Regina Formaran,OU=PE</t>
   </si>
@@ -1037,12 +1037,6 @@
     <t>INSERT INTO `trainee_group` (`id`, `name`, `section`, `level`, `remarks`) VALUES</t>
   </si>
   <si>
-    <t>(1, 'Electronics', 'A', 1, NULL),</t>
-  </si>
-  <si>
-    <t>(2, 'Mechtronics', 'A', 1, NULL),</t>
-  </si>
-  <si>
     <t>Basic Electricity and System</t>
   </si>
   <si>
@@ -1412,7 +1406,10 @@
     <t>WELD</t>
   </si>
   <si>
-    <t>Welding &amp; Fabrication</t>
+    <t>INSERT INTO `instructor` (`id`, `id_number`, `first_name`, `last_name`, `note`) VALUES</t>
+  </si>
+  <si>
+    <t>Weldin &amp; Fabrication</t>
   </si>
 </sst>
 </file>
@@ -1907,13 +1904,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3015,7 +3015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -6294,10 +6294,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F69"/>
+  <dimension ref="B3:F69"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6307,32 +6307,35 @@
     <col min="6" max="6" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6">
+    <row r="3" spans="2:6">
       <c r="C3" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="2:6">
       <c r="C4" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="2:6">
       <c r="C5" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="2:6">
       <c r="C6" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="2:6">
       <c r="C7" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" t="s">
         <v>248</v>
       </c>
@@ -6346,10 +6349,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>100</v>
-      </c>
+    <row r="9" spans="2:6">
       <c r="B9" t="s">
         <v>231</v>
       </c>
@@ -6364,13 +6364,10 @@
       </c>
       <c r="F9" t="str">
         <f>CONCATENATE("(",A9,", ","'",B9,"', '",C9,"', ",E9,", '",D9," - Instructor'),")</f>
-        <v>(100, 'Abdulaziz', 'Abid Galm Al Hinai', 2017001, 'ELC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>101</v>
-      </c>
+        <v>(, 'Abdulaziz', 'Abid Galm Al Hinai', 2017001, 'ELC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" t="s">
         <v>231</v>
       </c>
@@ -6385,13 +6382,10 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" ref="F10:F69" si="0">CONCATENATE("(",A10,", ","'",B10,"', '",C10,"', ",E10,", '",D10," - Instructor'),")</f>
-        <v>(101, 'Abdulaziz', 'Jumah Al Shamaki', 2017002, 'RAC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>102</v>
-      </c>
+        <v>(, 'Abdulaziz', 'Jumah Al Shamaki', 2017002, 'RAC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" t="s">
         <v>230</v>
       </c>
@@ -6406,13 +6400,10 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>(102, 'Abdullah', 'Maher.Abdullah', 2017003, 'ELC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>103</v>
-      </c>
+        <v>(, 'Abdullah', 'Maher.Abdullah', 2017003, 'ELC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" t="s">
         <v>207</v>
       </c>
@@ -6427,13 +6418,10 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>(103, 'Abdurahiman', 'Puthan', 2017004, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>104</v>
-      </c>
+        <v>(, 'Abdurahiman', 'Puthan', 2017004, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" t="s">
         <v>198</v>
       </c>
@@ -6448,13 +6436,10 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>(104, 'Ahmed', 'Mahsob', 2017005, 'BUS - Instructor'),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>105</v>
-      </c>
+        <v>(, 'Ahmed', 'Mahsob', 2017005, 'BUS - Instructor'),</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" t="s">
         <v>198</v>
       </c>
@@ -6469,13 +6454,10 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>(105, 'Ahmed', 'AL-Maqbali', 2017006, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>106</v>
-      </c>
+        <v>(, 'Ahmed', 'AL-Maqbali', 2017006, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" t="s">
         <v>206</v>
       </c>
@@ -6490,13 +6472,10 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>(106, 'Ali', 'Mohammed Ali Salih', 2017007, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>107</v>
-      </c>
+        <v>(, 'Ali', 'Mohammed Ali Salih', 2017007, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
       <c r="B16" t="s">
         <v>232</v>
       </c>
@@ -6511,13 +6490,10 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>(107, 'Ammar', 'Bin Mosbah', 2017008, 'MECH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>108</v>
-      </c>
+        <v>(, 'Ammar', 'Bin Mosbah', 2017008, 'MECH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" t="s">
         <v>220</v>
       </c>
@@ -6532,13 +6508,10 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>(108, 'antonio', 'Buca', 2017009, 'PHY - Instructor'),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>109</v>
-      </c>
+        <v>(, 'antonio', 'Buca', 2017009, 'PHY - Instructor'),</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" t="s">
         <v>210</v>
       </c>
@@ -6553,13 +6526,10 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>(109, 'Aref', 'Al ajmi', 2017010, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>110</v>
-      </c>
+        <v>(, 'Aref', 'Al ajmi', 2017010, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" t="s">
         <v>202</v>
       </c>
@@ -6574,13 +6544,10 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>(110, 'Asma', 'AL-', 2017011, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>111</v>
-      </c>
+        <v>(, 'Asma', 'AL-', 2017011, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
       <c r="B20" t="s">
         <v>202</v>
       </c>
@@ -6595,13 +6562,10 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>(111, 'Asma', 'Al Farsi', 2017012, 'PHY - Instructor'),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>112</v>
-      </c>
+        <v>(, 'Asma', 'Al Farsi', 2017012, 'PHY - Instructor'),</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
       <c r="B21" t="s">
         <v>221</v>
       </c>
@@ -6616,13 +6580,10 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>(112, 'Ayeesha', 'Yasmin', 2017013, 'PHY - Instructor'),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
-        <v>113</v>
-      </c>
+        <v>(, 'Ayeesha', 'Yasmin', 2017013, 'PHY - Instructor'),</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
       <c r="B22" t="s">
         <v>218</v>
       </c>
@@ -6637,13 +6598,10 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>(113, 'Ayoub', 'Al Oufi', 2017014, 'MATH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>114</v>
-      </c>
+        <v>(, 'Ayoub', 'Al Oufi', 2017014, 'MATH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
       <c r="B23" t="s">
         <v>219</v>
       </c>
@@ -6658,13 +6616,10 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>(114, 'Bilal', 'Al Arqenah', 2017015, 'PHY - Instructor'),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>115</v>
-      </c>
+        <v>(, 'Bilal', 'Al Arqenah', 2017015, 'PHY - Instructor'),</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
       <c r="B24" t="s">
         <v>193</v>
       </c>
@@ -6679,13 +6634,10 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>(115, 'Carlo', 'Romion', 2017016, 'PE - Instructor'),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25">
-        <v>116</v>
-      </c>
+        <v>(, 'Carlo', 'Romion', 2017016, 'PE - Instructor'),</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
       <c r="B25" t="s">
         <v>223</v>
       </c>
@@ -6700,13 +6652,10 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>(116, 'Conrado', 'Torres', 2017017, 'ELX - Instructor'),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26">
-        <v>117</v>
-      </c>
+        <v>(, 'Conrado', 'Torres', 2017017, 'ELX - Instructor'),</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
       <c r="B26" t="s">
         <v>213</v>
       </c>
@@ -6721,13 +6670,10 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>(117, 'Ericson', 'Billedo', 2017018, 'IT - Instructor'),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27">
-        <v>118</v>
-      </c>
+        <v>(, 'Ericson', 'Billedo', 2017018, 'IT - Instructor'),</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
       <c r="B27" t="s">
         <v>227</v>
       </c>
@@ -6742,13 +6688,10 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>(118, 'Euclid', 'Santiago', 2017019, 'ELC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28">
-        <v>119</v>
-      </c>
+        <v>(, 'Euclid', 'Santiago', 2017019, 'ELC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
       <c r="B28" t="s">
         <v>224</v>
       </c>
@@ -6763,13 +6706,10 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>(119, 'Eulogio', 'Oderon', 2017020, 'ELX - Instructor'),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29">
-        <v>120</v>
-      </c>
+        <v>(, 'Eulogio', 'Oderon', 2017020, 'ELX - Instructor'),</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
       <c r="B29" t="s">
         <v>208</v>
       </c>
@@ -6784,13 +6724,10 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>(120, 'Fatma', 'AL-Blushi', 2017021, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30">
-        <v>121</v>
-      </c>
+        <v>(, 'Fatma', 'AL-Blushi', 2017021, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
       <c r="B30" t="s">
         <v>208</v>
       </c>
@@ -6805,13 +6742,10 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>(121, 'Fatma', 'Al Balushi', 2017022, 'IT - Instructor'),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31">
-        <v>122</v>
-      </c>
+        <v>(, 'Fatma', 'Al Balushi', 2017022, 'IT - Instructor'),</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
       <c r="B31" t="s">
         <v>233</v>
       </c>
@@ -6826,13 +6760,10 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>(122, 'Ghalib', 'Al Amri', 2017023, 'MECH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32">
-        <v>123</v>
-      </c>
+        <v>(, 'Ghalib', 'Al Amri', 2017023, 'MECH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
       <c r="B32" t="s">
         <v>229</v>
       </c>
@@ -6847,13 +6778,10 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>(123, 'Hermogenes', 'Baculo', 2017024, 'ELC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33">
-        <v>124</v>
-      </c>
+        <v>(, 'Hermogenes', 'Baculo', 2017024, 'ELC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
       <c r="B33" t="s">
         <v>225</v>
       </c>
@@ -6868,13 +6796,10 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>(124, 'Ibrahim', 'Saif Said Al Mawaali', 2017025, 'ELC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34">
-        <v>125</v>
-      </c>
+        <v>(, 'Ibrahim', 'Saif Said Al Mawaali', 2017025, 'ELC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
       <c r="B34" t="s">
         <v>226</v>
       </c>
@@ -6889,13 +6814,10 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>(125, 'Ignatius', 'Rodrigues', 2017026, 'ELC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35">
-        <v>126</v>
-      </c>
+        <v>(, 'Ignatius', 'Rodrigues', 2017026, 'ELC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
       <c r="B35" t="s">
         <v>216</v>
       </c>
@@ -6910,13 +6832,10 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>(126, 'Jaffar', 'Al. Bahrani', 2017027, 'MATH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36">
-        <v>127</v>
-      </c>
+        <v>(, 'Jaffar', 'Al. Bahrani', 2017027, 'MATH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
       <c r="B36" t="s">
         <v>240</v>
       </c>
@@ -6931,13 +6850,10 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>(127, 'Jenier', 'Galarpe', 2017028, 'WEL - Instructor'),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37">
-        <v>128</v>
-      </c>
+        <v>(, 'Jenier', 'Galarpe', 2017028, 'WEL - Instructor'),</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
       <c r="B37" t="s">
         <v>201</v>
       </c>
@@ -6952,13 +6868,10 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>(128, 'Julie', 'Mathew Senil', 2017029, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
-        <v>129</v>
-      </c>
+        <v>(, 'Julie', 'Mathew Senil', 2017029, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
       <c r="B38" t="s">
         <v>238</v>
       </c>
@@ -6973,13 +6886,10 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>(129, 'Juluis', 'Dabon', 2017030, 'RAC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39">
-        <v>130</v>
-      </c>
+        <v>(, 'Juluis', 'Dabon', 2017030, 'RAC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
       <c r="B39" t="s">
         <v>194</v>
       </c>
@@ -6994,13 +6904,10 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>(130, 'Kannan', 'subash chandra bose', 2017031, 'DRW - Instructor'),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40">
-        <v>131</v>
-      </c>
+        <v>(, 'Kannan', 'subash chandra bose', 2017031, 'DRW - Instructor'),</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
       <c r="B40" t="s">
         <v>228</v>
       </c>
@@ -7015,13 +6922,10 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>(131, 'Karunadas', 'Parakunnath', 2017032, 'ELC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>132</v>
-      </c>
+        <v>(, 'Karunadas', 'Parakunnath', 2017032, 'ELC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
       <c r="B41" t="s">
         <v>235</v>
       </c>
@@ -7036,13 +6940,10 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>(132, 'Macario', 'Barredo', 2017033, 'MECH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42">
-        <v>133</v>
-      </c>
+        <v>(, 'Macario', 'Barredo', 2017033, 'MECH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
       <c r="B42" t="s">
         <v>205</v>
       </c>
@@ -7057,13 +6958,10 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>(133, 'Mansoor', 'Al Balushi', 2017034, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43">
-        <v>134</v>
-      </c>
+        <v>(, 'Mansoor', 'Al Balushi', 2017034, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
       <c r="B43" t="s">
         <v>203</v>
       </c>
@@ -7078,13 +6976,10 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>(134, 'Marwan', 'ahmed. Almamari', 2017035, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44">
-        <v>135</v>
-      </c>
+        <v>(, 'Marwan', 'ahmed. Almamari', 2017035, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
       <c r="B44" t="s">
         <v>209</v>
       </c>
@@ -7099,13 +6994,10 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>(135, 'Maryam', 'AL-Mamary', 2017036, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45">
-        <v>136</v>
-      </c>
+        <v>(, 'Maryam', 'AL-Mamary', 2017036, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
       <c r="B45" t="s">
         <v>197</v>
       </c>
@@ -7120,13 +7012,10 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>(136, 'Mohammed', 'Mahmoud Saliem', 2017037, 'BUS - Instructor'),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46">
-        <v>137</v>
-      </c>
+        <v>(, 'Mohammed', 'Mahmoud Saliem', 2017037, 'BUS - Instructor'),</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
       <c r="B46" t="s">
         <v>197</v>
       </c>
@@ -7141,13 +7030,10 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>(137, 'Mohammed', 'Nasser Abdullah Al Balushi', 2017038, 'BUS - Instructor'),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47">
-        <v>138</v>
-      </c>
+        <v>(, 'Mohammed', 'Nasser Abdullah Al Balushi', 2017038, 'BUS - Instructor'),</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
       <c r="B47" t="s">
         <v>197</v>
       </c>
@@ -7162,13 +7048,10 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>(138, 'Mohammed', 'Al-BAlushi', 2017039, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48">
-        <v>139</v>
-      </c>
+        <v>(, 'Mohammed', 'Al-BAlushi', 2017039, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
       <c r="B48" t="s">
         <v>197</v>
       </c>
@@ -7183,13 +7066,10 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>(139, 'Mohammed', 'Nabbhan Al Nabbhani', 2017040, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49">
-        <v>140</v>
-      </c>
+        <v>(, 'Mohammed', 'Nabbhan Al Nabbhani', 2017040, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
       <c r="B49" t="s">
         <v>197</v>
       </c>
@@ -7204,13 +7084,10 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>(140, 'Mohammed', 'ALNabhani', 2017041, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50">
-        <v>141</v>
-      </c>
+        <v>(, 'Mohammed', 'ALNabhani', 2017041, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
       <c r="B50" t="s">
         <v>197</v>
       </c>
@@ -7225,13 +7102,10 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>(141, 'Mohammed', 'Vaziruddin', 2017042, 'MATH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51">
-        <v>142</v>
-      </c>
+        <v>(, 'Mohammed', 'Vaziruddin', 2017042, 'MATH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
       <c r="B51" t="s">
         <v>236</v>
       </c>
@@ -7246,13 +7120,10 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>(142, 'mohammed', 'al-basyuni al-said al qal youbi', 2017043, 'RAC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
-        <v>143</v>
-      </c>
+        <v>(, 'mohammed', 'al-basyuni al-said al qal youbi', 2017043, 'RAC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
       <c r="B52" t="s">
         <v>197</v>
       </c>
@@ -7267,13 +7138,10 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>(143, 'Mohammed', 'Ramdan Salim', 2017044, 'WEL - Instructor'),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
-        <v>144</v>
-      </c>
+        <v>(, 'Mohammed', 'Ramdan Salim', 2017044, 'WEL - Instructor'),</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
       <c r="B53" t="s">
         <v>195</v>
       </c>
@@ -7288,13 +7156,10 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>(144, 'Mustafa', 'Metwally', 2017045, 'DRW - Instructor'),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
-        <v>145</v>
-      </c>
+        <v>(, 'Mustafa', 'Metwally', 2017045, 'DRW - Instructor'),</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
       <c r="B54" t="s">
         <v>217</v>
       </c>
@@ -7309,13 +7174,10 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>(145, 'NAGAPAVAN', '.N', 2017046, 'MATH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55">
-        <v>146</v>
-      </c>
+        <v>(, 'NAGAPAVAN', '.N', 2017046, 'MATH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
       <c r="B55" t="s">
         <v>234</v>
       </c>
@@ -7330,13 +7192,10 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>(146, 'Nasir', 'Al Hinai', 2017047, 'MECH - Instructor'),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56">
-        <v>147</v>
-      </c>
+        <v>(, 'Nasir', 'Al Hinai', 2017047, 'MECH - Instructor'),</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
       <c r="B56" t="s">
         <v>239</v>
       </c>
@@ -7351,13 +7210,10 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>(147, 'Norman', 'De Ocampo', 2017048, 'RAC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57">
-        <v>148</v>
-      </c>
+        <v>(, 'Norman', 'De Ocampo', 2017048, 'RAC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
       <c r="B57" t="s">
         <v>237</v>
       </c>
@@ -7372,13 +7228,10 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>(148, 'Osamah', 'Mohammad Ahmmad Al-Shobaki', 2017049, 'RAC - Instructor'),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58">
-        <v>149</v>
-      </c>
+        <v>(, 'Osamah', 'Mohammad Ahmmad Al-Shobaki', 2017049, 'RAC - Instructor'),</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
       <c r="B58" t="s">
         <v>199</v>
       </c>
@@ -7393,13 +7246,10 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>(149, 'Rajesh', 'Chaladath', 2017050, 'BUS - Instructor'),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59">
-        <v>150</v>
-      </c>
+        <v>(, 'Rajesh', 'Chaladath', 2017050, 'BUS - Instructor'),</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
       <c r="B59" t="s">
         <v>192</v>
       </c>
@@ -7414,13 +7264,10 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>(150, 'Regina', 'Formaran', 2017051, 'PE - Instructor'),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60">
-        <v>151</v>
-      </c>
+        <v>(, 'Regina', 'Formaran', 2017051, 'PE - Instructor'),</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
       <c r="B60" t="s">
         <v>196</v>
       </c>
@@ -7435,13 +7282,10 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>(151, 'Rojesb', 'Chaladatb', 2017052, 'DRW - Instructor'),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61">
-        <v>152</v>
-      </c>
+        <v>(, 'Rojesb', 'Chaladatb', 2017052, 'DRW - Instructor'),</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
       <c r="B61" t="s">
         <v>241</v>
       </c>
@@ -7456,13 +7300,10 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>(152, 'Rommel', 'A. Rosales', 2017053, 'WEL - Instructor'),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62">
-        <v>153</v>
-      </c>
+        <v>(, 'Rommel', 'A. Rosales', 2017053, 'WEL - Instructor'),</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
       <c r="B62" t="s">
         <v>211</v>
       </c>
@@ -7477,13 +7318,10 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>(153, 'Sajith', 'Bandara', 2017054, 'IT - Instructor'),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63">
-        <v>154</v>
-      </c>
+        <v>(, 'Sajith', 'Bandara', 2017054, 'IT - Instructor'),</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
       <c r="B63" t="s">
         <v>214</v>
       </c>
@@ -7498,13 +7336,10 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>(154, 'Sheikha', 'Ali Said Al-Badi', 2017055, 'IT - Instructor'),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64">
-        <v>155</v>
-      </c>
+        <v>(, 'Sheikha', 'Ali Said Al-Badi', 2017055, 'IT - Instructor'),</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
       <c r="B64" t="s">
         <v>204</v>
       </c>
@@ -7519,13 +7354,10 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>(155, 'Silpa', 'Sarah Abraham', 2017056, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65">
-        <v>156</v>
-      </c>
+        <v>(, 'Silpa', 'Sarah Abraham', 2017056, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
       <c r="B65" t="s">
         <v>242</v>
       </c>
@@ -7540,13 +7372,10 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v>(156, 'Taoufik', 'Ouelhazi', 2017057, 'WEL - Instructor'),</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66">
-        <v>157</v>
-      </c>
+        <v>(, 'Taoufik', 'Ouelhazi', 2017057, 'WEL - Instructor'),</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
       <c r="B66" t="s">
         <v>215</v>
       </c>
@@ -7561,13 +7390,10 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v>(157, 'Vara', 'Prasad Reddy Subbi Reddy', 2017058, 'IT - Instructor'),</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67">
-        <v>158</v>
-      </c>
+        <v>(, 'Vara', 'Prasad Reddy Subbi Reddy', 2017058, 'IT - Instructor'),</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
       <c r="B67" t="s">
         <v>212</v>
       </c>
@@ -7582,13 +7408,10 @@
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v>(158, 'Vijaya', 'kumar', 2017059, 'IT - Instructor'),</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68">
-        <v>159</v>
-      </c>
+        <v>(, 'Vijaya', 'kumar', 2017059, 'IT - Instructor'),</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
       <c r="B68" t="s">
         <v>200</v>
       </c>
@@ -7603,13 +7426,10 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" si="0"/>
-        <v>(159, 'vinay', 'kumar', 2017060, 'ENG - Instructor'),</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69">
-        <v>160</v>
-      </c>
+        <v>(, 'vinay', 'kumar', 2017060, 'ENG - Instructor'),</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
       <c r="B69" t="s">
         <v>222</v>
       </c>
@@ -7624,7 +7444,7 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" si="0"/>
-        <v>(160, 'William', 'Caniedo', 2017061, 'ELX - Instructor'),</v>
+        <v>(, 'William', 'Caniedo', 2017061, 'ELX - Instructor'),</v>
       </c>
     </row>
   </sheetData>
@@ -7632,6 +7452,7 @@
     <sortCondition ref="B8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7639,8 +7460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G38"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7693,9 +7514,7 @@
       <c r="D7" t="s">
         <v>328</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>336</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7">
       <c r="C8" t="s">
@@ -7704,9 +7523,7 @@
       <c r="D8" t="s">
         <v>331</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>337</v>
-      </c>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7">
       <c r="C9" t="s">
@@ -7718,19 +7535,19 @@
     </row>
     <row r="10" spans="2:7">
       <c r="F10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="F11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12">
         <v>136</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12" s="3">
@@ -7742,18 +7559,18 @@
       </c>
       <c r="F12" t="str">
         <f>CONCATENATE("Term ",D12," ",$F$11, " Trainees")</f>
-        <v>Term 1 Welding &amp; Fabrication Trainees</v>
+        <v>Term 1 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G12" t="str">
         <f>CONCATENATE("(",B12,",","'",$F$10,"-",D12,E12,"','",E12,"',",D12,",","'",F12,"'),")</f>
-        <v>(136,'WELD-1A','A',1,'Term 1 Welding &amp; Fabrication Trainees'),</v>
+        <v>(136,'WELD-1A','A',1,'Term 1 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13">
         <v>137</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="3">
         <f>C12</f>
         <v>1</v>
@@ -7763,18 +7580,18 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" ref="F13:F38" si="0">CONCATENATE("Term ",D13," ",$F$11, " Trainees")</f>
-        <v>Term 1 Welding &amp; Fabrication Trainees</v>
+        <v>Term 1 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ref="G13:G38" si="1">CONCATENATE("(",B13,",","'",$F$10,"-",D13,E13,"','",E13,"',",D13,",","'",F13,"'),")</f>
-        <v>(137,'WELD-1B','B',1,'Term 1 Welding &amp; Fabrication Trainees'),</v>
+        <v>(137,'WELD-1B','B',1,'Term 1 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14">
         <v>138</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="3">
         <f>C12</f>
         <v>1</v>
@@ -7784,531 +7601,531 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>Term 1 Welding &amp; Fabrication Trainees</v>
+        <v>Term 1 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>(138,'WELD-1C','C',1,'Term 1 Welding &amp; Fabrication Trainees'),</v>
+        <v>(138,'WELD-1C','C',1,'Term 1 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15">
         <v>139</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>2</v>
       </c>
       <c r="D15" s="3">
         <f>C15</f>
         <v>2</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="4" t="s">
         <v>332</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>Term 2 Welding &amp; Fabrication Trainees</v>
+        <v>Term 2 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>(139,'WELD-2A','A',2,'Term 2 Welding &amp; Fabrication Trainees'),</v>
+        <v>(139,'WELD-2A','A',2,'Term 2 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="B16">
         <v>140</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="3">
         <f>C15</f>
         <v>2</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>333</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>Term 2 Welding &amp; Fabrication Trainees</v>
+        <v>Term 2 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>(140,'WELD-2B','B',2,'Term 2 Welding &amp; Fabrication Trainees'),</v>
+        <v>(140,'WELD-2B','B',2,'Term 2 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17">
         <v>141</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="3">
         <f>C15</f>
         <v>2</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>334</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>Term 2 Welding &amp; Fabrication Trainees</v>
+        <v>Term 2 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>(141,'WELD-2C','C',2,'Term 2 Welding &amp; Fabrication Trainees'),</v>
+        <v>(141,'WELD-2C','C',2,'Term 2 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18">
         <v>142</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>3</v>
       </c>
       <c r="D18" s="3">
         <f>C18</f>
         <v>3</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>332</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>Term 3 Welding &amp; Fabrication Trainees</v>
+        <v>Term 3 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
-        <v>(142,'WELD-3A','A',3,'Term 3 Welding &amp; Fabrication Trainees'),</v>
+        <v>(142,'WELD-3A','A',3,'Term 3 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19">
         <v>143</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="3">
         <f>C18</f>
         <v>3</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>333</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>Term 3 Welding &amp; Fabrication Trainees</v>
+        <v>Term 3 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>(143,'WELD-3B','B',3,'Term 3 Welding &amp; Fabrication Trainees'),</v>
+        <v>(143,'WELD-3B','B',3,'Term 3 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20">
         <v>144</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="3">
         <f>C18</f>
         <v>3</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>334</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>Term 3 Welding &amp; Fabrication Trainees</v>
+        <v>Term 3 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
-        <v>(144,'WELD-3C','C',3,'Term 3 Welding &amp; Fabrication Trainees'),</v>
+        <v>(144,'WELD-3C','C',3,'Term 3 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="B21">
         <v>145</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="5">
         <v>4</v>
       </c>
       <c r="D21" s="3">
         <f>C21</f>
         <v>4</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>332</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>Term 4 Welding &amp; Fabrication Trainees</v>
+        <v>Term 4 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>(145,'WELD-4A','A',4,'Term 4 Welding &amp; Fabrication Trainees'),</v>
+        <v>(145,'WELD-4A','A',4,'Term 4 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22">
         <v>146</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="3">
         <f>C21</f>
         <v>4</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>332</v>
+      <c r="E22" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>Term 4 Welding &amp; Fabrication Trainees</v>
+        <v>Term 4 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>(146,'WELD-4A','A',4,'Term 4 Welding &amp; Fabrication Trainees'),</v>
+        <v>(146,'WELD-4B','B',4,'Term 4 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="23" spans="2:7">
       <c r="B23">
         <v>147</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="3">
         <f>C21</f>
         <v>4</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>333</v>
+      <c r="E23" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>Term 4 Welding &amp; Fabrication Trainees</v>
+        <v>Term 4 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>(147,'WELD-4B','B',4,'Term 4 Welding &amp; Fabrication Trainees'),</v>
+        <v>(147,'WELD-4C','C',4,'Term 4 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="24" spans="2:7">
       <c r="B24">
         <v>148</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="5">
         <v>5</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" ref="D24" si="2">C24</f>
         <v>5</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>334</v>
+      <c r="E24" s="4" t="s">
+        <v>332</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>Term 5 Welding &amp; Fabrication Trainees</v>
+        <v>Term 5 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>(148,'WELD-5C','C',5,'Term 5 Welding &amp; Fabrication Trainees'),</v>
+        <v>(148,'WELD-5A','A',5,'Term 5 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="25" spans="2:7">
       <c r="B25">
         <v>149</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="3">
         <f t="shared" ref="D25" si="3">C24</f>
         <v>5</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>332</v>
+      <c r="E25" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>Term 5 Welding &amp; Fabrication Trainees</v>
+        <v>Term 5 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
-        <v>(149,'WELD-5A','A',5,'Term 5 Welding &amp; Fabrication Trainees'),</v>
+        <v>(149,'WELD-5B','B',5,'Term 5 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26">
         <v>150</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="3">
         <f t="shared" ref="D26" si="4">C24</f>
         <v>5</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>333</v>
+      <c r="E26" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>Term 5 Welding &amp; Fabrication Trainees</v>
+        <v>Term 5 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
-        <v>(150,'WELD-5B','B',5,'Term 5 Welding &amp; Fabrication Trainees'),</v>
+        <v>(150,'WELD-5C','C',5,'Term 5 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="27" spans="2:7">
       <c r="B27">
         <v>151</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="5">
         <v>6</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27" si="5">C27</f>
         <v>6</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>334</v>
+      <c r="E27" s="4" t="s">
+        <v>332</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>Term 6 Welding &amp; Fabrication Trainees</v>
+        <v>Term 6 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
-        <v>(151,'WELD-6C','C',6,'Term 6 Welding &amp; Fabrication Trainees'),</v>
+        <v>(151,'WELD-6A','A',6,'Term 6 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="28" spans="2:7">
       <c r="B28">
         <v>152</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="3">
         <f t="shared" ref="D28" si="6">C27</f>
         <v>6</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>332</v>
+      <c r="E28" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>Term 6 Welding &amp; Fabrication Trainees</v>
+        <v>Term 6 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>(152,'WELD-6A','A',6,'Term 6 Welding &amp; Fabrication Trainees'),</v>
+        <v>(152,'WELD-6B','B',6,'Term 6 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="29" spans="2:7">
       <c r="B29">
         <v>153</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="3">
         <f t="shared" ref="D29" si="7">C27</f>
         <v>6</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>332</v>
+      <c r="E29" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>Term 6 Welding &amp; Fabrication Trainees</v>
+        <v>Term 6 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
-        <v>(153,'WELD-6A','A',6,'Term 6 Welding &amp; Fabrication Trainees'),</v>
+        <v>(153,'WELD-6C','C',6,'Term 6 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="30" spans="2:7">
       <c r="B30">
         <v>154</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="5">
         <v>7</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" ref="D30" si="8">C30</f>
         <v>7</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>333</v>
+      <c r="E30" s="4" t="s">
+        <v>332</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>Term 7 Welding &amp; Fabrication Trainees</v>
+        <v>Term 7 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>(154,'WELD-7B','B',7,'Term 7 Welding &amp; Fabrication Trainees'),</v>
+        <v>(154,'WELD-7A','A',7,'Term 7 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="31" spans="2:7">
       <c r="B31">
         <v>155</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="3">
         <f t="shared" ref="D31" si="9">C30</f>
         <v>7</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>334</v>
+      <c r="E31" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>Term 7 Welding &amp; Fabrication Trainees</v>
+        <v>Term 7 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
-        <v>(155,'WELD-7C','C',7,'Term 7 Welding &amp; Fabrication Trainees'),</v>
+        <v>(155,'WELD-7B','B',7,'Term 7 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="32" spans="2:7">
       <c r="B32">
         <v>156</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="3">
         <f t="shared" ref="D32" si="10">C30</f>
         <v>7</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>332</v>
+      <c r="E32" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>Term 7 Welding &amp; Fabrication Trainees</v>
+        <v>Term 7 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
-        <v>(156,'WELD-7A','A',7,'Term 7 Welding &amp; Fabrication Trainees'),</v>
+        <v>(156,'WELD-7C','C',7,'Term 7 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="33" spans="2:7">
       <c r="B33">
         <v>157</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="5">
         <v>8</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" ref="D33" si="11">C33</f>
         <v>8</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>333</v>
+      <c r="E33" s="4" t="s">
+        <v>332</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>Term 8 Welding &amp; Fabrication Trainees</v>
+        <v>Term 8 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
-        <v>(157,'WELD-8B','B',8,'Term 8 Welding &amp; Fabrication Trainees'),</v>
+        <v>(157,'WELD-8A','A',8,'Term 8 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="34" spans="2:7">
       <c r="B34">
         <v>158</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="3">
         <f t="shared" ref="D34" si="12">C33</f>
         <v>8</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>334</v>
+      <c r="E34" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>Term 8 Welding &amp; Fabrication Trainees</v>
+        <v>Term 8 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
-        <v>(158,'WELD-8C','C',8,'Term 8 Welding &amp; Fabrication Trainees'),</v>
+        <v>(158,'WELD-8B','B',8,'Term 8 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="35" spans="2:7">
       <c r="B35">
         <v>159</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="3">
         <f t="shared" ref="D35" si="13">C33</f>
         <v>8</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>332</v>
+      <c r="E35" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>Term 8 Welding &amp; Fabrication Trainees</v>
+        <v>Term 8 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
-        <v>(159,'WELD-8A','A',8,'Term 8 Welding &amp; Fabrication Trainees'),</v>
+        <v>(159,'WELD-8C','C',8,'Term 8 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="36" spans="2:7">
       <c r="B36">
         <v>160</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="5">
         <v>9</v>
       </c>
       <c r="D36" s="3">
         <f t="shared" ref="D36" si="14">C36</f>
         <v>9</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="4" t="s">
         <v>332</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>Term 9 Welding &amp; Fabrication Trainees</v>
+        <v>Term 9 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
-        <v>(160,'WELD-9A','A',9,'Term 9 Welding &amp; Fabrication Trainees'),</v>
+        <v>(160,'WELD-9A','A',9,'Term 9 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="37" spans="2:7">
       <c r="B37">
         <v>161</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="3">
         <f t="shared" ref="D37" si="15">C36</f>
         <v>9</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="4" t="s">
         <v>333</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>Term 9 Welding &amp; Fabrication Trainees</v>
+        <v>Term 9 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
-        <v>(161,'WELD-9B','B',9,'Term 9 Welding &amp; Fabrication Trainees'),</v>
+        <v>(161,'WELD-9B','B',9,'Term 9 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="38" spans="2:7">
       <c r="B38">
         <v>162</v>
       </c>
-      <c r="C38" s="4"/>
+      <c r="C38" s="5"/>
       <c r="D38" s="3">
         <f t="shared" ref="D38" si="16">C36</f>
         <v>9</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="4" t="s">
         <v>334</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>Term 9 Welding &amp; Fabrication Trainees</v>
+        <v>Term 9 Weldin &amp; Fabrication Trainees</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
-        <v>(162,'WELD-9C','C',9,'Term 9 Welding &amp; Fabrication Trainees'),</v>
+        <v>(162,'WELD-9C','C',9,'Term 9 Weldin &amp; Fabrication Trainees'),</v>
       </c>
     </row>
     <row r="43" spans="2:7">
@@ -8359,8 +8176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F66"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8373,12 +8190,12 @@
   <sheetData>
     <row r="1" spans="2:9">
       <c r="D1" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="2:9">
       <c r="D2" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="2:9">
@@ -8386,13 +8203,13 @@
     </row>
     <row r="4" spans="2:9">
       <c r="C4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -8400,10 +8217,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -8418,10 +8235,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -8436,10 +8253,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -8454,10 +8271,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -8472,10 +8289,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -8490,10 +8307,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E10">
         <v>6</v>
@@ -8508,10 +8325,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -8526,10 +8343,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -8544,10 +8361,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -8562,10 +8379,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -8580,10 +8397,10 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D15" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -8598,10 +8415,10 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -8616,10 +8433,10 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D17" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -8634,10 +8451,10 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D18" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -8652,10 +8469,10 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D19" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -8670,10 +8487,10 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D20" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -8688,10 +8505,10 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D21" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -8706,10 +8523,10 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D22" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -8724,10 +8541,10 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -8742,10 +8559,10 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D24" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -8760,10 +8577,10 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D25" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E25">
         <v>7</v>
@@ -8778,10 +8595,10 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E26">
         <v>5</v>
@@ -8796,10 +8613,10 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -8814,10 +8631,10 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D28" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -8832,10 +8649,10 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D29" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -8850,10 +8667,10 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D30" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -8868,10 +8685,10 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D31" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -8886,10 +8703,10 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D32" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -8904,10 +8721,10 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D33" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -8922,10 +8739,10 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D34" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -8940,10 +8757,10 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -8958,10 +8775,10 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D36" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -8976,10 +8793,10 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D37" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E37">
         <v>5</v>
@@ -8994,10 +8811,10 @@
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D38" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -9012,10 +8829,10 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D39" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -9030,10 +8847,10 @@
         <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D40" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -9048,10 +8865,10 @@
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D41" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -9066,10 +8883,10 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D42" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -9084,10 +8901,10 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D43" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -9102,10 +8919,10 @@
         <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D44" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -9120,10 +8937,10 @@
         <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D45" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -9138,10 +8955,10 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D46" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -9156,10 +8973,10 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D47" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -9174,10 +8991,10 @@
         <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D48" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E48">
         <v>3</v>
@@ -9192,10 +9009,10 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D49" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -9210,10 +9027,10 @@
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D50" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -9228,10 +9045,10 @@
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D51" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E51">
         <v>4</v>
@@ -9246,10 +9063,10 @@
         <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D52" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -9264,10 +9081,10 @@
         <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D53" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -9282,10 +9099,10 @@
         <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D54" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -9300,10 +9117,10 @@
         <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D55" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E55">
         <v>4</v>
@@ -9318,10 +9135,10 @@
         <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D56" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -9336,10 +9153,10 @@
         <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D57" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -9354,10 +9171,10 @@
         <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D58" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -9372,10 +9189,10 @@
         <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D59" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E59">
         <v>3</v>
@@ -9390,10 +9207,10 @@
         <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D60" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -9408,10 +9225,10 @@
         <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D61" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E61">
         <v>3</v>
@@ -9426,10 +9243,10 @@
         <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D62" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E62">
         <v>7</v>
@@ -9444,10 +9261,10 @@
         <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D63" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E63">
         <v>8</v>
@@ -9462,10 +9279,10 @@
         <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D64" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E64">
         <v>5</v>
@@ -9480,10 +9297,10 @@
         <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D65" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E65">
         <v>12</v>
@@ -9498,10 +9315,10 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D66" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E66">
         <v>9</v>

</xml_diff>

<commit_message>
GA now Fully Working
</commit_message>
<xml_diff>
--- a/csv/user.xlsx
+++ b/csv/user.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -6311,7 +6311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F70"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F7" sqref="F7:F70"/>
     </sheetView>
   </sheetViews>
@@ -6405,8 +6405,8 @@
         <v>259</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>(2,2017002,'Abdulaziz','Abid Galm Al Hinai','ELC Study Break'),</v>
+        <f>CONCATENATE("(",A10,",",B10,",'",C10,"','",D10,"','",E10," - Instructor'),")</f>
+        <v>(2,2017002,'Abdulaziz','Abid Galm Al Hinai','ELC - Instructor'),</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6426,8 +6426,8 @@
         <v>261</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>(3,2017003,'Abdulaziz','Jumah Al Shamaki','RAC Study Break'),</v>
+        <f t="shared" ref="F11:F70" si="1">CONCATENATE("(",A11,",",B11,",'",C11,"','",D11,"','",E11," - Instructor'),")</f>
+        <v>(3,2017003,'Abdulaziz','Jumah Al Shamaki','RAC - Instructor'),</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6447,8 +6447,8 @@
         <v>259</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>(4,2017004,'Abdullah','Maher.Abdullah','ELC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(4,2017004,'Abdullah','Maher.Abdullah','ELC - Instructor'),</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6468,8 +6468,8 @@
         <v>254</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>(5,2017005,'Abdurahiman','Puthan','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(5,2017005,'Abdurahiman','Puthan','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -6489,8 +6489,8 @@
         <v>253</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>(6,2017006,'Ahmed','Mahsob','BUS Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(6,2017006,'Ahmed','Mahsob','BUS - Instructor'),</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -6510,8 +6510,8 @@
         <v>254</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>(7,2017007,'Ahmed','AL-Maqbali','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(7,2017007,'Ahmed','AL-Maqbali','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6531,8 +6531,8 @@
         <v>254</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>(8,2017008,'Ali','Mohammed Ali Salih','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(8,2017008,'Ali','Mohammed Ali Salih','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -6552,8 +6552,8 @@
         <v>260</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>(9,2017009,'Ammar','Bin Mosbah','MECH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(9,2017009,'Ammar','Bin Mosbah','MECH - Instructor'),</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6573,8 +6573,8 @@
         <v>257</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>(10,2017010,'antonio','Buca','PHY Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(10,2017010,'antonio','Buca','PHY - Instructor'),</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -6594,8 +6594,8 @@
         <v>254</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>(11,2017011,'Aref','Al ajmi','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(11,2017011,'Aref','Al ajmi','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -6615,8 +6615,8 @@
         <v>254</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>(12,2017012,'Asma','AL-','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(12,2017012,'Asma','AL-','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6636,8 +6636,8 @@
         <v>257</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>(13,2017013,'Asma','Al Farsi','PHY Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(13,2017013,'Asma','Al Farsi','PHY - Instructor'),</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -6657,8 +6657,8 @@
         <v>257</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>(14,2017014,'Ayeesha','Yasmin','PHY Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(14,2017014,'Ayeesha','Yasmin','PHY - Instructor'),</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -6678,8 +6678,8 @@
         <v>256</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>(15,2017015,'Ayoub','Al Oufi','MATH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(15,2017015,'Ayoub','Al Oufi','MATH - Instructor'),</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6699,8 +6699,8 @@
         <v>257</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>(16,2017016,'Bilal','Al Arqenah','PHY Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(16,2017016,'Bilal','Al Arqenah','PHY - Instructor'),</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -6720,8 +6720,8 @@
         <v>251</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v>(17,2017017,'Carlo','Romion','PE Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(17,2017017,'Carlo','Romion','PE - Instructor'),</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -6741,8 +6741,8 @@
         <v>258</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v>(18,2017018,'Conrado','Torres','ELX Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(18,2017018,'Conrado','Torres','ELX - Instructor'),</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -6762,8 +6762,8 @@
         <v>255</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v>(19,2017019,'Ericson','Billedo','IT Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(19,2017019,'Ericson','Billedo','IT - Instructor'),</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -6783,8 +6783,8 @@
         <v>259</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>(20,2017020,'Euclid','Santiago','ELC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(20,2017020,'Euclid','Santiago','ELC - Instructor'),</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -6804,8 +6804,8 @@
         <v>258</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v>(21,2017021,'Eulogio','Oderon','ELX Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(21,2017021,'Eulogio','Oderon','ELX - Instructor'),</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -6825,8 +6825,8 @@
         <v>254</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v>(22,2017022,'Fatma','AL-Blushi','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(22,2017022,'Fatma','AL-Blushi','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6846,8 +6846,8 @@
         <v>255</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v>(23,2017023,'Fatma','Al Balushi','IT Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(23,2017023,'Fatma','Al Balushi','IT - Instructor'),</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6867,8 +6867,8 @@
         <v>260</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v>(24,2017024,'Ghalib','Al Amri','MECH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(24,2017024,'Ghalib','Al Amri','MECH - Instructor'),</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -6888,8 +6888,8 @@
         <v>259</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="0"/>
-        <v>(25,2017025,'Hermogenes','Baculo','ELC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(25,2017025,'Hermogenes','Baculo','ELC - Instructor'),</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -6909,8 +6909,8 @@
         <v>259</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v>(26,2017026,'Ibrahim','Saif Said Al Mawaali','ELC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(26,2017026,'Ibrahim','Saif Said Al Mawaali','ELC - Instructor'),</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6930,8 +6930,8 @@
         <v>259</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="0"/>
-        <v>(27,2017027,'Ignatius','Rodrigues','ELC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(27,2017027,'Ignatius','Rodrigues','ELC - Instructor'),</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -6951,8 +6951,8 @@
         <v>256</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="0"/>
-        <v>(28,2017028,'Jaffar','Al. Bahrani','MATH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(28,2017028,'Jaffar','Al. Bahrani','MATH - Instructor'),</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6972,8 +6972,8 @@
         <v>262</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="0"/>
-        <v>(29,2017029,'Jenier','Galarpe','WEL Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(29,2017029,'Jenier','Galarpe','WEL - Instructor'),</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6993,8 +6993,8 @@
         <v>254</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="0"/>
-        <v>(30,2017030,'Julie','Mathew Senil','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(30,2017030,'Julie','Mathew Senil','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -7014,8 +7014,8 @@
         <v>261</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="0"/>
-        <v>(31,2017031,'Juluis','Dabon','RAC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(31,2017031,'Juluis','Dabon','RAC - Instructor'),</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -7035,8 +7035,8 @@
         <v>252</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="0"/>
-        <v>(32,2017032,'Kannan','subash chandra bose','DRW Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(32,2017032,'Kannan','subash chandra bose','DRW - Instructor'),</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -7056,8 +7056,8 @@
         <v>259</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="0"/>
-        <v>(33,2017033,'Karunadas','Parakunnath','ELC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(33,2017033,'Karunadas','Parakunnath','ELC - Instructor'),</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -7077,8 +7077,8 @@
         <v>260</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="0"/>
-        <v>(34,2017034,'Macario','Barredo','MECH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(34,2017034,'Macario','Barredo','MECH - Instructor'),</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -7098,8 +7098,8 @@
         <v>254</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="0"/>
-        <v>(35,2017035,'Mansoor','Al Balushi','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(35,2017035,'Mansoor','Al Balushi','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -7119,8 +7119,8 @@
         <v>254</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v>(36,2017036,'Marwan','ahmed. Almamari','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(36,2017036,'Marwan','ahmed. Almamari','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -7140,8 +7140,8 @@
         <v>254</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v>(37,2017037,'Maryam','AL-Mamary','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(37,2017037,'Maryam','AL-Mamary','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -7161,8 +7161,8 @@
         <v>253</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="0"/>
-        <v>(38,2017038,'Mohammed','Mahmoud Saliem','BUS Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(38,2017038,'Mohammed','Mahmoud Saliem','BUS - Instructor'),</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -7182,8 +7182,8 @@
         <v>253</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="0"/>
-        <v>(39,2017039,'Mohammed','Nasser Abdullah Al Balushi','BUS Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(39,2017039,'Mohammed','Nasser Abdullah Al Balushi','BUS - Instructor'),</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -7203,8 +7203,8 @@
         <v>254</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="0"/>
-        <v>(40,2017040,'Mohammed','Al-BAlushi','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(40,2017040,'Mohammed','Al-BAlushi','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -7224,8 +7224,8 @@
         <v>254</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="0"/>
-        <v>(41,2017041,'Mohammed','Nabbhan Al Nabbhani','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(41,2017041,'Mohammed','Nabbhan Al Nabbhani','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -7245,8 +7245,8 @@
         <v>254</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="0"/>
-        <v>(42,2017042,'Mohammed','ALNabhani','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(42,2017042,'Mohammed','ALNabhani','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -7266,8 +7266,8 @@
         <v>256</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="0"/>
-        <v>(43,2017043,'Mohammed','Vaziruddin','MATH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(43,2017043,'Mohammed','Vaziruddin','MATH - Instructor'),</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -7287,8 +7287,8 @@
         <v>261</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="0"/>
-        <v>(44,2017044,'mohammed','al-basyuni al-said al qal youbi','RAC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(44,2017044,'mohammed','al-basyuni al-said al qal youbi','RAC - Instructor'),</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -7308,8 +7308,8 @@
         <v>262</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="0"/>
-        <v>(45,2017045,'Mohammed','Ramdan Salim','WEL Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(45,2017045,'Mohammed','Ramdan Salim','WEL - Instructor'),</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -7329,8 +7329,8 @@
         <v>252</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="0"/>
-        <v>(46,2017046,'Mustafa','Metwally','DRW Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(46,2017046,'Mustafa','Metwally','DRW - Instructor'),</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -7350,8 +7350,8 @@
         <v>256</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="0"/>
-        <v>(47,2017047,'NAGAPAVAN','.N','MATH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(47,2017047,'NAGAPAVAN','.N','MATH - Instructor'),</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -7371,8 +7371,8 @@
         <v>260</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="0"/>
-        <v>(48,2017048,'Nasir','Al Hinai','MECH Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(48,2017048,'Nasir','Al Hinai','MECH - Instructor'),</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -7392,8 +7392,8 @@
         <v>261</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="0"/>
-        <v>(49,2017049,'Norman','De Ocampo','RAC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(49,2017049,'Norman','De Ocampo','RAC - Instructor'),</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -7413,8 +7413,8 @@
         <v>261</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="0"/>
-        <v>(50,2017050,'Osamah','Mohammad Ahmmad Al-Shobaki','RAC Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(50,2017050,'Osamah','Mohammad Ahmmad Al-Shobaki','RAC - Instructor'),</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -7434,8 +7434,8 @@
         <v>253</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="0"/>
-        <v>(51,2017051,'Rajesh','Chaladath','BUS Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(51,2017051,'Rajesh','Chaladath','BUS - Instructor'),</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -7455,8 +7455,8 @@
         <v>251</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="0"/>
-        <v>(52,2017052,'Regina','Formaran','PE Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(52,2017052,'Regina','Formaran','PE - Instructor'),</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -7476,8 +7476,8 @@
         <v>252</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="0"/>
-        <v>(53,2017053,'Rojesb','Chaladatb','DRW Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(53,2017053,'Rojesb','Chaladatb','DRW - Instructor'),</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -7497,8 +7497,8 @@
         <v>262</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="0"/>
-        <v>(54,2017054,'Rommel','A. Rosales','WEL Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(54,2017054,'Rommel','A. Rosales','WEL - Instructor'),</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -7518,8 +7518,8 @@
         <v>255</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="0"/>
-        <v>(55,2017055,'Sajith','Bandara','IT Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(55,2017055,'Sajith','Bandara','IT - Instructor'),</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -7539,8 +7539,8 @@
         <v>255</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="0"/>
-        <v>(56,2017056,'Sheikha','Ali Said Al-Badi','IT Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(56,2017056,'Sheikha','Ali Said Al-Badi','IT - Instructor'),</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -7560,8 +7560,8 @@
         <v>254</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>(57,2017057,'Silpa','Sarah Abraham','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(57,2017057,'Silpa','Sarah Abraham','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -7581,8 +7581,8 @@
         <v>262</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="0"/>
-        <v>(58,2017058,'Taoufik','Ouelhazi','WEL Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(58,2017058,'Taoufik','Ouelhazi','WEL - Instructor'),</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -7602,8 +7602,8 @@
         <v>255</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="0"/>
-        <v>(59,2017059,'Vara','Prasad Reddy Subbi Reddy','IT Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(59,2017059,'Vara','Prasad Reddy Subbi Reddy','IT - Instructor'),</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -7623,8 +7623,8 @@
         <v>255</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="0"/>
-        <v>(60,2017060,'Vijaya','kumar','IT Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(60,2017060,'Vijaya','kumar','IT - Instructor'),</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -7644,8 +7644,8 @@
         <v>254</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="0"/>
-        <v>(61,2017061,'vinay','kumar','ENG Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(61,2017061,'vinay','kumar','ENG - Instructor'),</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -7665,8 +7665,8 @@
         <v>258</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="0"/>
-        <v>(62,2017062,'William','Caniedo','ELX Study Break'),</v>
+        <f t="shared" si="1"/>
+        <v>(62,2017062,'William','Caniedo','ELX - Instructor'),</v>
       </c>
     </row>
   </sheetData>
@@ -8398,7 +8398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F5" sqref="F5:F66"/>
     </sheetView>
   </sheetViews>
@@ -8451,7 +8451,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="str">
-        <f>CONCATENATE("(",B5,",'",C5,"','",D5,"',",E5,",''),")</f>
+        <f t="shared" ref="F5:F36" si="0">CONCATENATE("(",B5,",'",C5,"','",D5,"',",E5,",''),")</f>
         <v>(1,'BBSSM 1101','PRINCIPLES OF MARKETING ',6,''),</v>
       </c>
     </row>
@@ -8469,7 +8469,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="str">
-        <f>CONCATENATE("(",B6,",'",C6,"','",D6,"',",E6,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(2,'BBSSM 1102','INTRODUCTION TO SELLING ',6,''),</v>
       </c>
     </row>
@@ -8487,7 +8487,7 @@
         <v>6</v>
       </c>
       <c r="F7" t="str">
-        <f>CONCATENATE("(",B7,",'",C7,"','",D7,"',",E7,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(3,'BBSSM 1103','ECONOMICS',6,''),</v>
       </c>
     </row>
@@ -8505,7 +8505,7 @@
         <v>6</v>
       </c>
       <c r="F8" t="str">
-        <f>CONCATENATE("(",B8,",'",C8,"','",D8,"',",E8,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(4,'BBSSM 1201','BUSINESS ETHICS',6,''),</v>
       </c>
     </row>
@@ -8523,7 +8523,7 @@
         <v>6</v>
       </c>
       <c r="F9" t="str">
-        <f>CONCATENATE("(",B9,",'",C9,"','",D9,"',",E9,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(5,'BBSSM 1202','ADVERTISIMENT &amp; PROMOTION',6,''),</v>
       </c>
     </row>
@@ -8541,7 +8541,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="str">
-        <f>CONCATENATE("(",B10,",'",C10,"','",D10,"',",E10,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(6,'BBSSM 1203','CONSUMER BEHAVIOR ',6,''),</v>
       </c>
     </row>
@@ -8559,7 +8559,7 @@
         <v>6</v>
       </c>
       <c r="F11" t="str">
-        <f>CONCATENATE("(",B11,",'",C11,"','",D11,"',",E11,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(7,'BBSSM 1204','BUSINESS RESEARCH METHODS',6,''),</v>
       </c>
     </row>
@@ -8577,7 +8577,7 @@
         <v>6</v>
       </c>
       <c r="F12" t="str">
-        <f>CONCATENATE("(",B12,",'",C12,"','",D12,"',",E12,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(8,'BBSSM 2101','DIRECT MARKETING ',6,''),</v>
       </c>
     </row>
@@ -8595,7 +8595,7 @@
         <v>6</v>
       </c>
       <c r="F13" t="str">
-        <f>CONCATENATE("(",B13,",'",C13,"','",D13,"',",E13,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(9,'BBSSM 2102','RETAILING MANAGEMENT ',6,''),</v>
       </c>
     </row>
@@ -8613,7 +8613,7 @@
         <v>6</v>
       </c>
       <c r="F14" t="str">
-        <f>CONCATENATE("(",B14,",'",C14,"','",D14,"',",E14,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(10,'BBSSM 2103','RETAIL PRICING STRAGEGIES ',6,''),</v>
       </c>
     </row>
@@ -8631,7 +8631,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="str">
-        <f>CONCATENATE("(",B15,",'",C15,"','",D15,"',",E15,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(11,'BBSSM 2104','PROFESSIONAL SELLING ',6,''),</v>
       </c>
     </row>
@@ -8649,7 +8649,7 @@
         <v>6</v>
       </c>
       <c r="F16" t="str">
-        <f>CONCATENATE("(",B16,",'",C16,"','",D16,"',",E16,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(12,'BBSSM 2201','CUSTOMER RELATIONSHIP MGT.',6,''),</v>
       </c>
     </row>
@@ -8667,7 +8667,7 @@
         <v>10</v>
       </c>
       <c r="F17" t="str">
-        <f>CONCATENATE("(",B17,",'",C17,"','",D17,"',",E17,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(13,'BBSSM 2201x','MANAGEMENT AND ORGANIZATION ',10,''),</v>
       </c>
     </row>
@@ -8685,7 +8685,7 @@
         <v>10</v>
       </c>
       <c r="F18" t="str">
-        <f>CONCATENATE("(",B18,",'",C18,"','",D18,"',",E18,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(14,'BBSSM 2204','MARKETING COMMUINCATION',10,''),</v>
       </c>
     </row>
@@ -8703,7 +8703,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="str">
-        <f>CONCATENATE("(",B19,",'",C19,"','",D19,"',",E19,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(15,'BBSSM 2204x','GRADUATION PROJECT ',10,''),</v>
       </c>
     </row>
@@ -8721,7 +8721,7 @@
         <v>4</v>
       </c>
       <c r="F20" t="str">
-        <f>CONCATENATE("(",B20,",'",C20,"','",D20,"',",E20,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(16,'CHEM 1101','Chemistry 1',4,''),</v>
       </c>
     </row>
@@ -8739,7 +8739,7 @@
         <v>4</v>
       </c>
       <c r="F21" t="str">
-        <f>CONCATENATE("(",B21,",'",C21,"','",D21,"',",E21,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(17,'CHEM 1202','Chemistry 2',4,''),</v>
       </c>
     </row>
@@ -8757,7 +8757,7 @@
         <v>10</v>
       </c>
       <c r="F22" t="str">
-        <f>CONCATENATE("(",B22,",'",C22,"','",D22,"',",E22,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(18,'EECIM 1101','Basic Electricity and System',10,''),</v>
       </c>
     </row>
@@ -8775,7 +8775,7 @@
         <v>10</v>
       </c>
       <c r="F23" t="str">
-        <f>CONCATENATE("(",B23,",'",C23,"','",D23,"',",E23,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(19,'EECIM 1102','Basic Electronics and Circuits',10,''),</v>
       </c>
     </row>
@@ -8793,7 +8793,7 @@
         <v>10</v>
       </c>
       <c r="F24" t="str">
-        <f>CONCATENATE("(",B24,",'",C24,"','",D24,"',",E24,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(20,'EECIM 1103','Fundamental Digital Electronics Circuits',10,''),</v>
       </c>
     </row>
@@ -8811,7 +8811,7 @@
         <v>7</v>
       </c>
       <c r="F25" t="str">
-        <f>CONCATENATE("(",B25,",'",C25,"','",D25,"',",E25,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(21,'EECIM 1203','ELX-?',7,''),</v>
       </c>
     </row>
@@ -8829,7 +8829,7 @@
         <v>5</v>
       </c>
       <c r="F26" t="str">
-        <f>CONCATENATE("(",B26,",'",C26,"','",D26,"',",E26,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(22,'EECIM 1204','Installation, Servicing Audio-Video Systems',5,''),</v>
       </c>
     </row>
@@ -8847,7 +8847,7 @@
         <v>10</v>
       </c>
       <c r="F27" t="str">
-        <f>CONCATENATE("(",B27,",'",C27,"','",D27,"',",E27,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(23,'EECIM 1205','Switched-Mode Power Supplies &amp; Autovolt Power',10,''),</v>
       </c>
     </row>
@@ -8865,7 +8865,7 @@
         <v>10</v>
       </c>
       <c r="F28" t="str">
-        <f>CONCATENATE("(",B28,",'",C28,"','",D28,"',",E28,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(24,'EECIM 1206','Electronics Devices Servicing 1',10,''),</v>
       </c>
     </row>
@@ -8883,7 +8883,7 @@
         <v>5</v>
       </c>
       <c r="F29" t="str">
-        <f>CONCATENATE("(",B29,",'",C29,"','",D29,"',",E29,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(25,'EECIM 1305','ELX-?',5,''),</v>
       </c>
     </row>
@@ -8901,7 +8901,7 @@
         <v>10</v>
       </c>
       <c r="F30" t="str">
-        <f>CONCATENATE("(",B30,",'",C30,"','",D30,"',",E30,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(26,'EECIM 2107','Personal Computers and Multimedia Devices',10,''),</v>
       </c>
     </row>
@@ -8919,7 +8919,7 @@
         <v>10</v>
       </c>
       <c r="F31" t="str">
-        <f>CONCATENATE("(",B31,",'",C31,"','",D31,"',",E31,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(27,'EECIM 2108','Computer System Data Comm. &amp; Internetworking',10,''),</v>
       </c>
     </row>
@@ -8937,7 +8937,7 @@
         <v>10</v>
       </c>
       <c r="F32" t="str">
-        <f>CONCATENATE("(",B32,",'",C32,"','",D32,"',",E32,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(28,'EECIM 2109','Graduation Project 1',10,''),</v>
       </c>
     </row>
@@ -8955,7 +8955,7 @@
         <v>10</v>
       </c>
       <c r="F33" t="str">
-        <f>CONCATENATE("(",B33,",'",C33,"','",D33,"',",E33,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(29,'EECIM 2210','Security Alarm systems',10,''),</v>
       </c>
     </row>
@@ -8973,7 +8973,7 @@
         <v>10</v>
       </c>
       <c r="F34" t="str">
-        <f>CONCATENATE("(",B34,",'",C34,"','",D34,"',",E34,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(30,'EECIM 2211','Electronics Devices Servicing 2',10,''),</v>
       </c>
     </row>
@@ -8991,7 +8991,7 @@
         <v>10</v>
       </c>
       <c r="F35" t="str">
-        <f>CONCATENATE("(",B35,",'",C35,"','",D35,"',",E35,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(31,'EECIM 2212','Graduation Project 2',10,''),</v>
       </c>
     </row>
@@ -9009,7 +9009,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="str">
-        <f>CONCATENATE("(",B36,",'",C36,"','",D36,"',",E36,",''),")</f>
+        <f t="shared" si="0"/>
         <v>(32,'EELIHW 1101','Health and Safety Precautions',1,''),</v>
       </c>
     </row>
@@ -9027,7 +9027,7 @@
         <v>5</v>
       </c>
       <c r="F37" t="str">
-        <f>CONCATENATE("(",B37,",'",C37,"','",D37,"',",E37,",''),")</f>
+        <f t="shared" ref="F37:F68" si="1">CONCATENATE("(",B37,",'",C37,"','",D37,"',",E37,",''),")</f>
         <v>(33,'EELIHW 1102','Basic Electricity(AC/DC) &amp;Electrical Code',5,''),</v>
       </c>
     </row>
@@ -9045,7 +9045,7 @@
         <v>5</v>
       </c>
       <c r="F38" t="str">
-        <f>CONCATENATE("(",B38,",'",C38,"','",D38,"',",E38,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(34,'EELIHW 1103','Tools, Instruments, Electric wires and cable works',5,''),</v>
       </c>
     </row>
@@ -9063,7 +9063,7 @@
         <v>4</v>
       </c>
       <c r="F39" t="str">
-        <f>CONCATENATE("(",B39,",'",C39,"','",D39,"',",E39,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(35,'EELIHW 1204','Basic Electronics',4,''),</v>
       </c>
     </row>
@@ -9081,7 +9081,7 @@
         <v>10</v>
       </c>
       <c r="F40" t="str">
-        <f>CONCATENATE("(",B40,",'",C40,"','",D40,"',",E40,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(36,'EELIHW 1205','Electrical-Circuits and Protection Devices',10,''),</v>
       </c>
     </row>
@@ -9099,7 +9099,7 @@
         <v>10</v>
       </c>
       <c r="F41" t="str">
-        <f>CONCATENATE("(",B41,",'",C41,"','",D41,"',",E41,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(37,'EELIHW 1206','Three Phase Principles',10,''),</v>
       </c>
     </row>
@@ -9117,7 +9117,7 @@
         <v>10</v>
       </c>
       <c r="F42" t="str">
-        <f>CONCATENATE("(",B42,",'",C42,"','",D42,"',",E42,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(38,'EENDR 1101','Engineering Drawing 1',10,''),</v>
       </c>
     </row>
@@ -9135,7 +9135,7 @@
         <v>10</v>
       </c>
       <c r="F43" t="str">
-        <f>CONCATENATE("(",B43,",'",C43,"','",D43,"',",E43,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(39,'EENDR 1202','Engineering Drawing 2',10,''),</v>
       </c>
     </row>
@@ -9153,7 +9153,7 @@
         <v>3</v>
       </c>
       <c r="F44" t="str">
-        <f>CONCATENATE("(",B44,",'",C44,"','",D44,"',",E44,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(40,'ENG 1101','TECHNICAL WRITING ',3,''),</v>
       </c>
     </row>
@@ -9171,7 +9171,7 @@
         <v>3</v>
       </c>
       <c r="F45" t="str">
-        <f>CONCATENATE("(",B45,",'",C45,"','",D45,"',",E45,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(41,'ENG 1202','TECHNICAL COMMUNICATION  ',3,''),</v>
       </c>
     </row>
@@ -9189,7 +9189,7 @@
         <v>10</v>
       </c>
       <c r="F46" t="str">
-        <f>CONCATENATE("(",B46,",'",C46,"','",D46,"',",E46,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(42,'ENTRP 1202','ENTREPRENEURSHIP',10,''),</v>
       </c>
     </row>
@@ -9207,7 +9207,7 @@
         <v>3</v>
       </c>
       <c r="F47" t="str">
-        <f>CONCATENATE("(",B47,",'",C47,"','",D47,"',",E47,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(43,'ENTRP 1101','Entrepreneurship 1',3,''),</v>
       </c>
     </row>
@@ -9225,7 +9225,7 @@
         <v>3</v>
       </c>
       <c r="F48" t="str">
-        <f>CONCATENATE("(",B48,",'",C48,"','",D48,"',",E48,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(44,'ENTRP 1203','Entrepreneurship 2',3,''),</v>
       </c>
     </row>
@@ -9243,7 +9243,7 @@
         <v>4</v>
       </c>
       <c r="F49" t="str">
-        <f>CONCATENATE("(",B49,",'",C49,"','",D49,"',",E49,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(45,'INBS 1202','E- COMMERCE ',4,''),</v>
       </c>
     </row>
@@ -9261,7 +9261,7 @@
         <v>4</v>
       </c>
       <c r="F50" t="str">
-        <f>CONCATENATE("(",B50,",'",C50,"','",D50,"',",E50,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(46,'INTE 1101 ','ADVANCED IT SKILLS ',4,''),</v>
       </c>
     </row>
@@ -9279,7 +9279,7 @@
         <v>4</v>
       </c>
       <c r="F51" t="str">
-        <f>CONCATENATE("(",B51,",'",C51,"','",D51,"',",E51,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(47,'INTE 1202','INTRODUCTION TO C++ Programming',4,''),</v>
       </c>
     </row>
@@ -9297,7 +9297,7 @@
         <v>4</v>
       </c>
       <c r="F52" t="str">
-        <f>CONCATENATE("(",B52,",'",C52,"','",D52,"',",E52,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(48,'MTBS 1202','BUSINESS MATHIMATICS',4,''),</v>
       </c>
     </row>
@@ -9315,7 +9315,7 @@
         <v>4</v>
       </c>
       <c r="F53" t="str">
-        <f>CONCATENATE("(",B53,",'",C53,"','",D53,"',",E53,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(49,'MTCL 1101','Calculus',4,''),</v>
       </c>
     </row>
@@ -9333,7 +9333,7 @@
         <v>4</v>
       </c>
       <c r="F54" t="str">
-        <f>CONCATENATE("(",B54,",'",C54,"','",D54,"',",E54,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(50,'MTCL 1202','Engineering Mathematics',4,''),</v>
       </c>
     </row>
@@ -9351,7 +9351,7 @@
         <v>4</v>
       </c>
       <c r="F55" t="str">
-        <f>CONCATENATE("(",B55,",'",C55,"','",D55,"',",E55,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(51,'MTST 1101','STATISTICS ',4,''),</v>
       </c>
     </row>
@@ -9369,7 +9369,7 @@
         <v>4</v>
       </c>
       <c r="F56" t="str">
-        <f>CONCATENATE("(",B56,",'",C56,"','",D56,"',",E56,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(52,'PHYS 1101','Physics 1',4,''),</v>
       </c>
     </row>
@@ -9387,7 +9387,7 @@
         <v>4</v>
       </c>
       <c r="F57" t="str">
-        <f>CONCATENATE("(",B57,",'",C57,"','",D57,"',",E57,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(53,'PHYS 1202','Physics 2',4,''),</v>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
         <v>10</v>
       </c>
       <c r="F58" t="str">
-        <f>CONCATENATE("(",B58,",'",C58,"','",D58,"',",E58,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(54,'PRMG 1101','ENTREPRENEURSHIP',10,''),</v>
       </c>
     </row>
@@ -9423,7 +9423,7 @@
         <v>3</v>
       </c>
       <c r="F59" t="str">
-        <f>CONCATENATE("(",B59,",'",C59,"','",D59,"',",E59,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(55,'PUENG 2101','Public Speaking',3,''),</v>
       </c>
     </row>
@@ -9441,7 +9441,7 @@
         <v>3</v>
       </c>
       <c r="F60" t="str">
-        <f>CONCATENATE("(",B60,",'",C60,"','",D60,"',",E60,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(56,'TCENG 1202','Technical Communication',3,''),</v>
       </c>
     </row>
@@ -9459,7 +9459,7 @@
         <v>3</v>
       </c>
       <c r="F61" t="str">
-        <f>CONCATENATE("(",B61,",'",C61,"','",D61,"',",E61,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(57,'TWENG 1101','TECHNICAL WRINTING ',3,''),</v>
       </c>
     </row>
@@ -9477,7 +9477,7 @@
         <v>7</v>
       </c>
       <c r="F62" t="str">
-        <f>CONCATENATE("(",B62,",'",C62,"','",D62,"',",E62,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(58,'EELIHW 1203','EELIHW 1203',7,''),</v>
       </c>
     </row>
@@ -9495,7 +9495,7 @@
         <v>8</v>
       </c>
       <c r="F63" t="str">
-        <f>CONCATENATE("(",B63,",'",C63,"','",D63,"',",E63,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(59,'EELIHW 2107','EELIHW 2107',8,''),</v>
       </c>
     </row>
@@ -9513,7 +9513,7 @@
         <v>5</v>
       </c>
       <c r="F64" t="str">
-        <f>CONCATENATE("(",B64,",'",C64,"','",D64,"',",E64,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(60,'EELIHW 2108','EELIHW 2108',5,''),</v>
       </c>
     </row>
@@ -9531,7 +9531,7 @@
         <v>12</v>
       </c>
       <c r="F65" t="str">
-        <f>CONCATENATE("(",B65,",'",C65,"','",D65,"',",E65,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(61,'EELIHW 2209','EELIHW 2209',12,''),</v>
       </c>
     </row>
@@ -9549,7 +9549,7 @@
         <v>9</v>
       </c>
       <c r="F66" t="str">
-        <f>CONCATENATE("(",B66,",'",C66,"','",D66,"',",E66,",''),")</f>
+        <f t="shared" si="1"/>
         <v>(62,'EELIHW 2210','EELIHW 2210',9,''),</v>
       </c>
     </row>

</xml_diff>